<commit_message>
CameraChangePos at the beginning
</commit_message>
<xml_diff>
--- a/GameDesign/ExcelData/Map_Data.xlsx
+++ b/GameDesign/ExcelData/Map_Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspace\University\ucsc\GAME 271\project-Nameless Hill\NamelessHill-Temp\NamelessHill\GameDesign\ExcelData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B87CCE3-C3DF-4E11-8EED-51BBB3740F53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A344DBF-F8FF-4EA0-BC41-01BB09CF5B4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="792" yWindow="1044" windowWidth="22248" windowHeight="9564" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="768" windowWidth="22248" windowHeight="9564" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="19">
   <si>
     <t>long</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -92,6 +92,14 @@
   </si>
   <si>
     <t>FinalLevel</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cameraPos</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[-10,30]</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -429,10 +437,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:J4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -440,11 +448,11 @@
     <col min="1" max="1" width="8.88671875" style="2"/>
     <col min="2" max="2" width="13.44140625" style="2" customWidth="1"/>
     <col min="3" max="4" width="18.44140625" style="2" customWidth="1"/>
-    <col min="5" max="8" width="26.44140625" style="2" customWidth="1"/>
-    <col min="9" max="9" width="24.21875" style="2" customWidth="1"/>
+    <col min="5" max="9" width="26.44140625" style="2" customWidth="1"/>
+    <col min="10" max="10" width="24.21875" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -470,10 +478,13 @@
         <v>15</v>
       </c>
       <c r="I1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="J1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -499,10 +510,13 @@
         <v>14</v>
       </c>
       <c r="I2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J2" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>0</v>
       </c>
@@ -527,11 +541,14 @@
       <c r="H3" s="2">
         <v>720</v>
       </c>
-      <c r="I3" s="2">
+      <c r="I3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="J3" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>1</v>
       </c>
@@ -556,7 +573,10 @@
       <c r="H4" s="2">
         <v>720</v>
       </c>
-      <c r="I4" s="2">
+      <c r="I4" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="J4" s="2">
         <v>0</v>
       </c>
     </row>

</xml_diff>